<commit_message>
Now table column names show in reports
Now the renamed column names for data tables show in reports and the preview

This means that you can now create a report 100% in another language other than English, while all the rfswarm screens are not language enabled at least the reports generated can be

Issue #104
</commit_message>
<xml_diff>
--- a/Tests/Demo/results/20230320_185055_demo/20230320_185055_demo.xlsx
+++ b/Tests/Demo/results/20230320_185055_demo/20230320_185055_demo.xlsx
@@ -8,11 +8,13 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cover" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="1 Template" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2 Test Result Summary" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="3 90%ile" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="4 test" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="5 Response vs Robots" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="1 toc" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2 Template" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="3 Test Result Summary" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="4 90%ile" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="5 test" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="6 Response vs Robots" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="7 DataTables" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -85,52 +87,52 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00557bdc"/>
+        <fgColor rgb="00dc42c3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="006c5c53"/>
+        <fgColor rgb="0018df77"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="005b973e"/>
+        <fgColor rgb="00ec10cb"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0088b225"/>
+        <fgColor rgb="00902b56"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00bbb2f9"/>
+        <fgColor rgb="00e3f011"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="009cc7b7"/>
+        <fgColor rgb="0029e36c"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00a8f351"/>
+        <fgColor rgb="00bd80da"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="002dbd20"/>
+        <fgColor rgb="0020a329"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ef71df"/>
+        <fgColor rgb="0025d07a"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00a0c965"/>
+        <fgColor rgb="000ea79c"/>
       </patternFill>
     </fill>
   </fills>
@@ -705,6 +707,129 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:A18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" ht="24" customHeight="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>1 toc</t>
+        </is>
+      </c>
+    </row>
+    <row r="2"/>
+    <row r="3">
+      <c r="A3">
+        <f>HYPERLINK(CONCATENATE("#'1 toc'!A",MATCH("1 toc",'1 toc'!A:A,0)),"1 toc")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <f>HYPERLINK(CONCATENATE("#'2 Template'!A",MATCH("2 Template",'2 Template'!A:A,0)),"2 Template")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <f>HYPERLINK(CONCATENATE("#'3 Test Result Summary'!A",MATCH("3 Test Result Summary",'3 Test Result Summary'!A:A,0)),"3 Test Result Summary")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <f>HYPERLINK(CONCATENATE("#'4 90%ile'!A",MATCH("4 90%ile",'4 90%ile'!A:A,0)),"4 90%ile")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <f>HYPERLINK(CONCATENATE("#'4 90%ile'!A",MATCH("4.1 90%ile Data",'4 90%ile'!A:A,0)),"4.1 90%ile Data")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <f>HYPERLINK(CONCATENATE("#'5 test'!A",MATCH("5 test",'5 test'!A:A,0)),"5 test")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <f>HYPERLINK(CONCATENATE("#'5 test'!A",MATCH("5.1 data left",'5 test'!A:A,0)),"5.1 data left")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <f>HYPERLINK(CONCATENATE("#'5 test'!A",MATCH("5.2 data right",'5 test'!A:A,0)),"5.2 data right")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <f>HYPERLINK(CONCATENATE("#'6 Response vs Robots'!A",MATCH("6 Response vs Robots",'6 Response vs Robots'!A:A,0)),"6 Response vs Robots")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <f>HYPERLINK(CONCATENATE("#'6 Response vs Robots'!A",MATCH("6.1 Robots",'6 Response vs Robots'!A:A,0)),"6.1 Robots")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <f>HYPERLINK(CONCATENATE("#'6 Response vs Robots'!A",MATCH("6.2 Response",'6 Response vs Robots'!A:A,0)),"6.2 Response")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <f>HYPERLINK(CONCATENATE("#'7 DataTables'!A",MATCH("7 DataTables",'7 DataTables'!A:A,0)),"7 DataTables")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <f>HYPERLINK(CONCATENATE("#'7 DataTables'!A",MATCH("7.1 Metric",'7 DataTables'!A:A,0)),"7.1 Metric")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <f>HYPERLINK(CONCATENATE("#'7 DataTables'!A",MATCH("7.2 ผลลัพธ์",'7 DataTables'!A:A,0)),"7.2 ผลลัพธ์")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <f>HYPERLINK(CONCATENATE("#'7 DataTables'!A",MATCH("7.3 Result Summary",'7 DataTables'!A:A,0)),"7.3 Result Summary")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <f>HYPERLINK(CONCATENATE("#'7 DataTables'!A",MATCH("7.4 SQL",'7 DataTables'!A:A,0)),"7.4 SQL")</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -716,7 +841,7 @@
     <row r="1" ht="24" customHeight="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>1 Template</t>
+          <t>2 Template</t>
         </is>
       </c>
     </row>
@@ -799,7 +924,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -828,7 +953,7 @@
     <row r="1" ht="24" customHeight="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>2 Test Result Summary</t>
+          <t>3 Test Result Summary</t>
         </is>
       </c>
     </row>
@@ -1074,7 +1199,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1100,7 +1225,7 @@
     <row r="1" ht="24" customHeight="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>3 90%ile</t>
+          <t>4 90%ile</t>
         </is>
       </c>
     </row>
@@ -1109,7 +1234,7 @@
     <row r="22" ht="24" customHeight="1">
       <c r="A22" s="7" t="inlineStr">
         <is>
-          <t>3.1 90%ile Data</t>
+          <t>4.1 90%ile Data</t>
         </is>
       </c>
     </row>
@@ -1285,7 +1410,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1312,7 +1437,7 @@
     <row r="1" ht="24" customHeight="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>4 test</t>
+          <t>5 test</t>
         </is>
       </c>
     </row>
@@ -1321,7 +1446,7 @@
     <row r="22" ht="24" customHeight="1">
       <c r="A22" s="7" t="inlineStr">
         <is>
-          <t>4.1 data left</t>
+          <t>5.1 data left</t>
         </is>
       </c>
     </row>
@@ -1480,7 +1605,7 @@
     <row r="29" ht="24" customHeight="1">
       <c r="A29" s="7" t="inlineStr">
         <is>
-          <t>4.2 data right</t>
+          <t>5.2 data right</t>
         </is>
       </c>
     </row>
@@ -1583,7 +1708,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1610,7 +1735,7 @@
     <row r="1" ht="24" customHeight="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
-          <t>5 Response vs Robots</t>
+          <t>6 Response vs Robots</t>
         </is>
       </c>
     </row>
@@ -1619,7 +1744,7 @@
     <row r="22" ht="24" customHeight="1">
       <c r="A22" s="7" t="inlineStr">
         <is>
-          <t>5.1 Robots</t>
+          <t>6.1 Robots</t>
         </is>
       </c>
     </row>
@@ -1740,7 +1865,7 @@
     <row r="28" ht="24" customHeight="1">
       <c r="A28" s="7" t="inlineStr">
         <is>
-          <t>5.2 Response</t>
+          <t>6.2 Response</t>
         </is>
       </c>
     </row>
@@ -1939,4 +2064,692 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="3" customWidth="1" min="1" max="1"/>
+    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="9.1" customWidth="1" min="3" max="3"/>
+    <col width="9.1" customWidth="1" min="4" max="4"/>
+    <col width="7.800000000000001" customWidth="1" min="5" max="5"/>
+    <col width="9.1" customWidth="1" min="6" max="6"/>
+    <col width="11.7" customWidth="1" min="7" max="7"/>
+    <col width="5.2" customWidth="1" min="8" max="8"/>
+    <col width="5.2" customWidth="1" min="9" max="9"/>
+    <col width="6.5" customWidth="1" min="10" max="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="24" customHeight="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>7 DataTables</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="24" customHeight="1">
+      <c r="A2" s="7" t="inlineStr">
+        <is>
+          <t>7.1 Metric</t>
+        </is>
+      </c>
+    </row>
+    <row r="3"/>
+    <row r="4">
+      <c r="B4" s="5" t="inlineStr">
+        <is>
+          <t>เมตริกหลัก</t>
+        </is>
+      </c>
+      <c r="C4" s="5" t="inlineStr">
+        <is>
+          <t>ชื่อตัวแทน</t>
+        </is>
+      </c>
+      <c r="D4" s="5" t="inlineStr">
+        <is>
+          <t>ขั้นต่ำ</t>
+        </is>
+      </c>
+      <c r="E4" s="5" t="inlineStr">
+        <is>
+          <t>เฉลี่ย</t>
+        </is>
+      </c>
+      <c r="F4" s="5" t="inlineStr">
+        <is>
+          <t>เปอร์เซ็นไทล์ที่ 90</t>
+        </is>
+      </c>
+      <c r="G4" s="5" t="inlineStr">
+        <is>
+          <t>ขีดสุด</t>
+        </is>
+      </c>
+      <c r="H4" s="5" t="inlineStr">
+        <is>
+          <t>ส่วนเบี่ยงเบนมาตรฐาน</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="12" t="n"/>
+      <c r="B5" s="6" t="inlineStr">
+        <is>
+          <t>Create Some Files</t>
+        </is>
+      </c>
+      <c r="C5" s="6" t="inlineStr">
+        <is>
+          <t>hp-elite-desk-800-g3</t>
+        </is>
+      </c>
+      <c r="D5" s="6" t="inlineStr">
+        <is>
+          <t>0.096</t>
+        </is>
+      </c>
+      <c r="E5" s="6" t="inlineStr">
+        <is>
+          <t>0.096</t>
+        </is>
+      </c>
+      <c r="F5" s="6" t="inlineStr">
+        <is>
+          <t>0.097</t>
+        </is>
+      </c>
+      <c r="G5" s="6" t="inlineStr">
+        <is>
+          <t>0.097</t>
+        </is>
+      </c>
+      <c r="H5" s="6" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="13" t="n"/>
+      <c r="B6" s="6" t="inlineStr">
+        <is>
+          <t>List Some Files</t>
+        </is>
+      </c>
+      <c r="C6" s="6" t="inlineStr">
+        <is>
+          <t>hp-elite-desk-800-g3</t>
+        </is>
+      </c>
+      <c r="D6" s="6" t="inlineStr">
+        <is>
+          <t>0.005</t>
+        </is>
+      </c>
+      <c r="E6" s="6" t="inlineStr">
+        <is>
+          <t>0.005</t>
+        </is>
+      </c>
+      <c r="F6" s="6" t="inlineStr">
+        <is>
+          <t>0.005</t>
+        </is>
+      </c>
+      <c r="G6" s="6" t="inlineStr">
+        <is>
+          <t>0.006</t>
+        </is>
+      </c>
+      <c r="H6" s="6" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="14" t="n"/>
+      <c r="B7" s="6" t="inlineStr">
+        <is>
+          <t>Remove Some Files</t>
+        </is>
+      </c>
+      <c r="C7" s="6" t="inlineStr">
+        <is>
+          <t>hp-elite-desk-800-g3</t>
+        </is>
+      </c>
+      <c r="D7" s="6" t="inlineStr">
+        <is>
+          <t>0.024</t>
+        </is>
+      </c>
+      <c r="E7" s="6" t="inlineStr">
+        <is>
+          <t>0.025</t>
+        </is>
+      </c>
+      <c r="F7" s="6" t="inlineStr">
+        <is>
+          <t>0.026</t>
+        </is>
+      </c>
+      <c r="G7" s="6" t="inlineStr">
+        <is>
+          <t>0.026</t>
+        </is>
+      </c>
+      <c r="H7" s="6" t="inlineStr">
+        <is>
+          <t>0.001</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="17" t="n"/>
+      <c r="B8" s="6" t="inlineStr">
+        <is>
+          <t>Show the RFS Variables</t>
+        </is>
+      </c>
+      <c r="C8" s="6" t="inlineStr">
+        <is>
+          <t>hp-elite-desk-800-g3</t>
+        </is>
+      </c>
+      <c r="D8" s="6" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="E8" s="6" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="F8" s="6" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="G8" s="6" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="H8" s="6" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="24" customHeight="1">
+      <c r="A10" s="7" t="inlineStr">
+        <is>
+          <t>7.2 ผลลัพธ์</t>
+        </is>
+      </c>
+    </row>
+    <row r="11"/>
+    <row r="12">
+      <c r="B12" s="5" t="inlineStr">
+        <is>
+          <t>ชื่อผลลัพธ์</t>
+        </is>
+      </c>
+      <c r="C12" s="5" t="inlineStr">
+        <is>
+          <t>ขั้นต่ำ</t>
+        </is>
+      </c>
+      <c r="D12" s="5" t="inlineStr">
+        <is>
+          <t>เฉลี่ย</t>
+        </is>
+      </c>
+      <c r="E12" s="5" t="inlineStr">
+        <is>
+          <t>เปอร์เซ็นไทล์ที่ 90</t>
+        </is>
+      </c>
+      <c r="F12" s="5" t="inlineStr">
+        <is>
+          <t>ขีดสุด</t>
+        </is>
+      </c>
+      <c r="G12" s="5" t="inlineStr">
+        <is>
+          <t>ส่วนเบี่ยงเบนมาตรฐาน</t>
+        </is>
+      </c>
+      <c r="H12" s="5" t="inlineStr">
+        <is>
+          <t>นับ</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="8" t="n"/>
+      <c r="B13" s="6" t="inlineStr">
+        <is>
+          <t>Create Some Files</t>
+        </is>
+      </c>
+      <c r="C13" s="6" t="inlineStr">
+        <is>
+          <t>0.076</t>
+        </is>
+      </c>
+      <c r="D13" s="6" t="inlineStr">
+        <is>
+          <t>0.085</t>
+        </is>
+      </c>
+      <c r="E13" s="6" t="inlineStr">
+        <is>
+          <t>0.096</t>
+        </is>
+      </c>
+      <c r="F13" s="6" t="inlineStr">
+        <is>
+          <t>0.117</t>
+        </is>
+      </c>
+      <c r="G13" s="6" t="inlineStr">
+        <is>
+          <t>0.009</t>
+        </is>
+      </c>
+      <c r="H13" s="6" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="9" t="n"/>
+      <c r="B14" s="6" t="inlineStr">
+        <is>
+          <t>List Some Files</t>
+        </is>
+      </c>
+      <c r="C14" s="6" t="inlineStr">
+        <is>
+          <t>0.001</t>
+        </is>
+      </c>
+      <c r="D14" s="6" t="inlineStr">
+        <is>
+          <t>0.004</t>
+        </is>
+      </c>
+      <c r="E14" s="6" t="inlineStr">
+        <is>
+          <t>0.005</t>
+        </is>
+      </c>
+      <c r="F14" s="6" t="inlineStr">
+        <is>
+          <t>0.006</t>
+        </is>
+      </c>
+      <c r="G14" s="6" t="inlineStr">
+        <is>
+          <t>0.001</t>
+        </is>
+      </c>
+      <c r="H14" s="6" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="10" t="n"/>
+      <c r="B15" s="6" t="inlineStr">
+        <is>
+          <t>Remove Some Files</t>
+        </is>
+      </c>
+      <c r="C15" s="6" t="inlineStr">
+        <is>
+          <t>0.008</t>
+        </is>
+      </c>
+      <c r="D15" s="6" t="inlineStr">
+        <is>
+          <t>0.016</t>
+        </is>
+      </c>
+      <c r="E15" s="6" t="inlineStr">
+        <is>
+          <t>0.024</t>
+        </is>
+      </c>
+      <c r="F15" s="6" t="inlineStr">
+        <is>
+          <t>0.027</t>
+        </is>
+      </c>
+      <c r="G15" s="6" t="inlineStr">
+        <is>
+          <t>0.007</t>
+        </is>
+      </c>
+      <c r="H15" s="6" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="11" t="n"/>
+      <c r="B16" s="6" t="inlineStr">
+        <is>
+          <t>Show the RFS Variables</t>
+        </is>
+      </c>
+      <c r="C16" s="6" t="inlineStr">
+        <is>
+          <t>0.003</t>
+        </is>
+      </c>
+      <c r="D16" s="6" t="inlineStr">
+        <is>
+          <t>0.007</t>
+        </is>
+      </c>
+      <c r="E16" s="6" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="F16" s="6" t="inlineStr">
+        <is>
+          <t>0.012</t>
+        </is>
+      </c>
+      <c r="G16" s="6" t="inlineStr">
+        <is>
+          <t>0.003</t>
+        </is>
+      </c>
+      <c r="H16" s="6" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="24" customHeight="1">
+      <c r="A18" s="7" t="inlineStr">
+        <is>
+          <t>7.3 Result Summary</t>
+        </is>
+      </c>
+    </row>
+    <row r="19"/>
+    <row r="20">
+      <c r="B20" s="5" t="inlineStr">
+        <is>
+          <t>Result Name</t>
+        </is>
+      </c>
+      <c r="C20" s="5" t="inlineStr">
+        <is>
+          <t>Minimum</t>
+        </is>
+      </c>
+      <c r="D20" s="5" t="inlineStr">
+        <is>
+          <t>Average</t>
+        </is>
+      </c>
+      <c r="E20" s="5" t="inlineStr">
+        <is>
+          <t>90%ile</t>
+        </is>
+      </c>
+      <c r="F20" s="5" t="inlineStr">
+        <is>
+          <t>Maximum</t>
+        </is>
+      </c>
+      <c r="G20" s="5" t="inlineStr">
+        <is>
+          <t>Std. Dev.</t>
+        </is>
+      </c>
+      <c r="H20" s="5" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="I20" s="5" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="J20" s="5" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="8" t="n"/>
+      <c r="B21" s="6" t="inlineStr">
+        <is>
+          <t>Create Some Files</t>
+        </is>
+      </c>
+      <c r="C21" s="6" t="inlineStr">
+        <is>
+          <t>0.076</t>
+        </is>
+      </c>
+      <c r="D21" s="6" t="inlineStr">
+        <is>
+          <t>0.085</t>
+        </is>
+      </c>
+      <c r="E21" s="6" t="inlineStr">
+        <is>
+          <t>0.096</t>
+        </is>
+      </c>
+      <c r="F21" s="6" t="inlineStr">
+        <is>
+          <t>0.117</t>
+        </is>
+      </c>
+      <c r="G21" s="6" t="inlineStr">
+        <is>
+          <t>0.009</t>
+        </is>
+      </c>
+      <c r="H21" s="6" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="I21" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J21" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="9" t="n"/>
+      <c r="B22" s="6" t="inlineStr">
+        <is>
+          <t>List Some Files</t>
+        </is>
+      </c>
+      <c r="C22" s="6" t="inlineStr">
+        <is>
+          <t>0.001</t>
+        </is>
+      </c>
+      <c r="D22" s="6" t="inlineStr">
+        <is>
+          <t>0.004</t>
+        </is>
+      </c>
+      <c r="E22" s="6" t="inlineStr">
+        <is>
+          <t>0.005</t>
+        </is>
+      </c>
+      <c r="F22" s="6" t="inlineStr">
+        <is>
+          <t>0.006</t>
+        </is>
+      </c>
+      <c r="G22" s="6" t="inlineStr">
+        <is>
+          <t>0.001</t>
+        </is>
+      </c>
+      <c r="H22" s="6" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="I22" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J22" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="10" t="n"/>
+      <c r="B23" s="6" t="inlineStr">
+        <is>
+          <t>Remove Some Files</t>
+        </is>
+      </c>
+      <c r="C23" s="6" t="inlineStr">
+        <is>
+          <t>0.008</t>
+        </is>
+      </c>
+      <c r="D23" s="6" t="inlineStr">
+        <is>
+          <t>0.016</t>
+        </is>
+      </c>
+      <c r="E23" s="6" t="inlineStr">
+        <is>
+          <t>0.024</t>
+        </is>
+      </c>
+      <c r="F23" s="6" t="inlineStr">
+        <is>
+          <t>0.027</t>
+        </is>
+      </c>
+      <c r="G23" s="6" t="inlineStr">
+        <is>
+          <t>0.007</t>
+        </is>
+      </c>
+      <c r="H23" s="6" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="I23" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J23" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="11" t="n"/>
+      <c r="B24" s="6" t="inlineStr">
+        <is>
+          <t>Show the RFS Variables</t>
+        </is>
+      </c>
+      <c r="C24" s="6" t="inlineStr">
+        <is>
+          <t>0.003</t>
+        </is>
+      </c>
+      <c r="D24" s="6" t="inlineStr">
+        <is>
+          <t>0.007</t>
+        </is>
+      </c>
+      <c r="E24" s="6" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="F24" s="6" t="inlineStr">
+        <is>
+          <t>0.012</t>
+        </is>
+      </c>
+      <c r="G24" s="6" t="inlineStr">
+        <is>
+          <t>0.003</t>
+        </is>
+      </c>
+      <c r="H24" s="6" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="I24" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J24" s="6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="26" ht="24" customHeight="1">
+      <c r="A26" s="7" t="inlineStr">
+        <is>
+          <t>7.4 SQL</t>
+        </is>
+      </c>
+    </row>
+    <row r="27"/>
+    <row r="29"/>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>